<commit_message>
Gathered more IMU data
</commit_message>
<xml_diff>
--- a/Documentation/Report/IMU fusion decision matrix.xlsx
+++ b/Documentation/Report/IMU fusion decision matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Uni\Year_2\Design_Project_2\EEEBalanceBug\Documentation\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9297D7-3201-4C6B-88F4-5777369A39EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FF9079-302A-4036-822E-2F989BDBD112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{AEAF3C4F-CC49-454A-BDAC-A062DB354F25}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Weight</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Robustness</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -117,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -125,17 +128,175 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -454,166 +615,173 @@
   <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.69140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    <row r="3" spans="2:7" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="19" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>-1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>-1</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="D5" s="15">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>3</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>-1</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
         <v>-1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>-1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>-1</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="D9" cm="1">
+      <c r="B9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="16" cm="1">
         <f t="array" ref="D9">SUM(C4:C8*D4:D8)</f>
         <v>-8</v>
       </c>
-      <c r="E9" cm="1">
+      <c r="E9" s="14" cm="1">
         <f t="array" ref="E9">SUM(C4:C8*E4:E8)</f>
         <v>-2</v>
       </c>
-      <c r="F9" cm="1">
+      <c r="F9" s="16" cm="1">
         <f t="array" ref="F9">SUM(C4:C8*F4:F8)</f>
         <v>-1</v>
       </c>
-      <c r="G9" cm="1">
+      <c r="G9" s="11" cm="1">
         <f t="array" ref="G9">SUM(G4:G8*C4:C8)</f>
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="D2:G2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:G8">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Added and updated report files
</commit_message>
<xml_diff>
--- a/Documentation/Report/IMU fusion decision matrix.xlsx
+++ b/Documentation/Report/IMU fusion decision matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Uni\Year_2\Design_Project_2\EEEBalanceBug\Documentation\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FF9079-302A-4036-822E-2F989BDBD112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A000B3DA-90C5-4E8A-9F6C-CCA9F22FC36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{AEAF3C4F-CC49-454A-BDAC-A062DB354F25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{AEAF3C4F-CC49-454A-BDAC-A062DB354F25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Weight</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Drift</t>
   </si>
   <si>
-    <t>Madgwick's Filter</t>
-  </si>
-  <si>
     <t>Extended Kalman Filter</t>
   </si>
   <si>
@@ -97,14 +94,28 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Complementary Filter</t>
+  </si>
+  <si>
+    <t>Madgwick Filter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -145,26 +156,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -250,52 +241,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -612,178 +599,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F8E860-DC74-4B3E-BAD1-A019D00882CF}">
-  <dimension ref="B2:G9"/>
+  <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D2" sqref="B2:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="11.69140625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="8" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="2:7" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="20" t="s">
+    <row r="3" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="19" t="s">
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
         <v>1</v>
       </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B4" s="8" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8">
-        <v>-1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
+      <c r="C8" s="5">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8">
-        <v>3</v>
-      </c>
-      <c r="D5" s="15">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="15">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="8">
-        <v>3</v>
-      </c>
-      <c r="D6" s="8">
-        <v>-1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B7" s="8" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8">
-        <v>-1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>-1</v>
-      </c>
-      <c r="F8" s="8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
-      <c r="B9" s="12" t="s">
-        <v>12</v>
-      </c>
       <c r="C9" s="13"/>
-      <c r="D9" s="16" cm="1">
+      <c r="D9" s="9" cm="1">
         <f t="array" ref="D9">SUM(C4:C8*D4:D8)</f>
+        <v>-7</v>
+      </c>
+      <c r="E9" s="9" cm="1">
+        <f t="array" ref="E9">SUM(C4:C8*E4:E8)</f>
         <v>-8</v>
       </c>
-      <c r="E9" s="14" cm="1">
-        <f t="array" ref="E9">SUM(C4:C8*E4:E8)</f>
+      <c r="F9" s="7" cm="1">
+        <f t="array" ref="F9">SUM(C4:C8*F4:F8)</f>
         <v>-2</v>
       </c>
-      <c r="F9" s="16" cm="1">
-        <f t="array" ref="F9">SUM(C4:C8*F4:F8)</f>
-        <v>-1</v>
-      </c>
-      <c r="G9" s="11" cm="1">
-        <f t="array" ref="G9">SUM(G4:G8*C4:C8)</f>
-        <v>9</v>
+      <c r="G9" s="9" cm="1">
+        <f t="array" ref="G9">SUM(C4:C8*G4:G8)</f>
+        <v>-1</v>
+      </c>
+      <c r="H9" s="6" cm="1">
+        <f t="array" ref="H9">SUM(H4:H8*C4:C8)</f>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D2:G2"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D2:H2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4:G8">
+  <conditionalFormatting sqref="E4:H8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:H8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>